<commit_message>
[TEST] change of sample1.xlsx and yaml defaults
</commit_message>
<xml_diff>
--- a/tests/testthat/files/sample1.xlsx
+++ b/tests/testthat/files/sample1.xlsx
@@ -105,13 +105,13 @@
 Parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">pret_a</t>
+    <t xml:space="preserve">slota_a</t>
   </si>
   <si>
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">slota_a</t>
+    <t xml:space="preserve">prefl_a</t>
   </si>
   <si>
     <t xml:space="preserve">Fluorescence Int.</t>
@@ -150,10 +150,10 @@
     <t xml:space="preserve">{'dynamic_threshold': False, 'relative_threshold': False, 'dynamic_smooth': 300, 'absolute_amplitude': 1.0, 'relative_amplitude_type': 'use std of noise', 'relative_amplitude': 1.0, 'interval': 50}</t>
   </si>
   <si>
-    <t xml:space="preserve">pret_b</t>
+    <t xml:space="preserve">slota_b</t>
   </si>
   <si>
-    <t xml:space="preserve">slota_b</t>
+    <t xml:space="preserve">prefl_b</t>
   </si>
   <si>
     <t xml:space="preserve">(306, 223)</t>
@@ -165,10 +165,10 @@
     <t xml:space="preserve">{'dynamic_threshold': False, 'relative_threshold': False, 'dynamic_smooth': 300, 'absolute_amplitude': 0.6, 'relative_amplitude_type': 'use std of noise', 'relative_amplitude': 1.0, 'interval': 50}</t>
   </si>
   <si>
-    <t xml:space="preserve">pret_c</t>
+    <t xml:space="preserve">slota_c</t>
   </si>
   <si>
-    <t xml:space="preserve">slota_c</t>
+    <t xml:space="preserve">prefl_c</t>
   </si>
   <si>
     <t xml:space="preserve">(145, 119)</t>
@@ -177,10 +177,10 @@
     <t xml:space="preserve">(111, 65)</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_a</t>
+    <t xml:space="preserve">slotb_a</t>
   </si>
   <si>
-    <t xml:space="preserve">slotb_a</t>
+    <t xml:space="preserve">postfl_a</t>
   </si>
   <si>
     <t xml:space="preserve">(330, 212)</t>
@@ -192,55 +192,55 @@
     <t xml:space="preserve">{'dynamic_threshold': False, 'relative_threshold': False, 'dynamic_smooth': 300, 'absolute_amplitude': 0.99, 'relative_amplitude_type': 'use std of noise', 'relative_amplitude': 1.0, 'interval': 50}</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_b</t>
-  </si>
-  <si>
     <t xml:space="preserve">slotb_b</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_c</t>
+    <t xml:space="preserve">postfl_b</t>
   </si>
   <si>
     <t xml:space="preserve">slotb_c</t>
   </si>
   <si>
+    <t xml:space="preserve">postfl_c</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">pret_a Train</t>
+    <t xml:space="preserve">prefl_a Train</t>
   </si>
   <si>
-    <t xml:space="preserve">pret_b Train</t>
+    <t xml:space="preserve">prefl_b Train</t>
   </si>
   <si>
-    <t xml:space="preserve">pret_c Train</t>
+    <t xml:space="preserve">prefl_c Train</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_a Train</t>
+    <t xml:space="preserve">postfl_a Train</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_b Train</t>
+    <t xml:space="preserve">postfl_b Train</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_c Train</t>
+    <t xml:space="preserve">postfl_c Train</t>
   </si>
   <si>
-    <t xml:space="preserve">pret_a Time of Peak (s) </t>
+    <t xml:space="preserve">prefl_a Time of Peak (s) </t>
   </si>
   <si>
-    <t xml:space="preserve">pret_b Time of Peak (s) </t>
+    <t xml:space="preserve">prefl_b Time of Peak (s) </t>
   </si>
   <si>
-    <t xml:space="preserve">pret_c Time of Peak (s) </t>
+    <t xml:space="preserve">prefl_c Time of Peak (s) </t>
   </si>
   <si>
-    <t xml:space="preserve">posta_a Time of Peak (s)</t>
+    <t xml:space="preserve">postfl_a Time of Peak (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_b Time of Peak (s)</t>
+    <t xml:space="preserve">postfl_b Time of Peak (s)</t>
   </si>
   <si>
-    <t xml:space="preserve">posta_c Time of Peak (s)</t>
+    <t xml:space="preserve">postfl_c Time of Peak (s)</t>
   </si>
 </sst>
 </file>
@@ -350,10 +350,10 @@
   <dimension ref="A1:U1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="J1:O3 A4"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59"/>
   </cols>
@@ -873,10 +873,10 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J1:O3 A1"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.52"/>
   </cols>
@@ -886,22 +886,22 @@
         <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1323,10 +1323,10 @@
   <dimension ref="A1:AI301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1:O3"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
global data crop; yaml remove unknown entries
</commit_message>
<xml_diff>
--- a/tests/testthat/files/sample1.xlsx
+++ b/tests/testthat/files/sample1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -353,7 +353,7 @@
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59"/>
   </cols>
@@ -872,11 +872,11 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.52"/>
   </cols>
@@ -1322,11 +1322,11 @@
   </sheetPr>
   <dimension ref="A1:AI301"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA24" activeCellId="0" sqref="AA24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
refactor TimeSlots, add more tests
* for mormalization testing modify sample files
</commit_message>
<xml_diff>
--- a/tests/testthat/files/sample1.xlsx
+++ b/tests/testthat/files/sample1.xlsx
@@ -350,10 +350,10 @@
   <dimension ref="A1:U1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="1" sqref="K2:M11 D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59"/>
   </cols>
@@ -870,13 +870,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2:M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.52"/>
   </cols>
@@ -909,13 +909,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.39228763</v>
+        <v>1.39228763</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.004714953</v>
+        <v>1.004714953</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.38953294</v>
+        <v>1.38953294</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>5.13654</v>
@@ -926,19 +926,22 @@
       <c r="G2" s="2" t="n">
         <v>5.515072</v>
       </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>0.1667</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.24045541</v>
+        <v>1.24045541</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.078318426</v>
+        <v>1.078318426</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.00410776</v>
+        <v>1.00410776</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>5.985954</v>
@@ -949,19 +952,22 @@
       <c r="G3" s="2" t="n">
         <v>5.418916</v>
       </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>0.3333</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.19479356</v>
+        <v>1.19479356</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.232332971</v>
+        <v>1.232332971</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.3566395</v>
+        <v>1.3566395</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>5.143817</v>
@@ -972,19 +978,22 @@
       <c r="G4" s="2" t="n">
         <v>5.896739</v>
       </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>0.5</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.40140614</v>
+        <v>1.40140614</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.417854419</v>
+        <v>1.417854419</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.1188747</v>
+        <v>1.1188747</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>5.783946</v>
@@ -995,19 +1004,22 @@
       <c r="G5" s="2" t="n">
         <v>5.017766</v>
       </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>0.6667</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.42688169</v>
+        <v>1.42688169</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.147947728</v>
+        <v>1.147947728</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.07352416</v>
+        <v>1.07352416</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>5.421845</v>
@@ -1018,19 +1030,22 @@
       <c r="G6" s="2" t="n">
         <v>5.866483</v>
       </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>0.8333</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.01686389</v>
+        <v>1.01686389</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.499702264</v>
+        <v>1.499702264</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.0174374</v>
+        <v>1.0174374</v>
       </c>
       <c r="E7" s="2" t="n">
         <v>5.963843</v>
@@ -1041,19 +1056,22 @@
       <c r="G7" s="2" t="n">
         <v>5.208876</v>
       </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.30861763</v>
+        <v>1.30861763</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.143142674</v>
+        <v>1.143142674</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.3688987</v>
+        <v>1.3688987</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>5.5849</v>
@@ -1064,19 +1082,22 @@
       <c r="G8" s="2" t="n">
         <v>5.372709</v>
       </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>1.1667</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.24628327</v>
+        <v>1.24628327</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.348686883</v>
+        <v>1.348686883</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0.32073118</v>
+        <v>1.32073118</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>5.913995</v>
@@ -1087,19 +1108,22 @@
       <c r="G9" s="2" t="n">
         <v>5.282218</v>
       </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>1.3333</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.20736767</v>
+        <v>1.20736767</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.05970239</v>
+        <v>1.05970239</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.26301483</v>
+        <v>1.26301483</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>5.977099</v>
@@ -1110,19 +1134,22 @@
       <c r="G10" s="2" t="n">
         <v>5.725983</v>
       </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>1.5</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.1851074</v>
+        <v>1.1851074</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.49167509</v>
+        <v>1.49167509</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.19415956</v>
+        <v>1.19415956</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>5.239595</v>
@@ -1133,6 +1160,9 @@
       <c r="G11" s="2" t="n">
         <v>5.101058</v>
       </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -1323,10 +1353,10 @@
   <dimension ref="A1:AI301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA24" activeCellId="0" sqref="AA24"/>
+      <selection pane="topLeft" activeCell="AA24" activeCellId="1" sqref="K2:M11 AA24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
   </cols>

</xml_diff>